<commit_message>
Added examples of constaints
</commit_message>
<xml_diff>
--- a/app/config/tables/TEST/forms/TEST/TEST.xlsx
+++ b/app/config/tables/TEST/forms/TEST/TEST.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555DE266-0589-45E4-AFC4-C93661FEF6E8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE44CDE9-EBDC-4146-8880-3899EB125530}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-2100" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="281">
   <si>
     <t>setting_name</t>
   </si>
@@ -876,6 +877,15 @@
   </si>
   <si>
     <t>Differencen var: {{calculates.diffInYears}} år.</t>
+  </si>
+  <si>
+    <t>constraint</t>
+  </si>
+  <si>
+    <t>display.constraint_message.text.english</t>
+  </si>
+  <si>
+    <t>display.constraint_message.text</t>
   </si>
 </sst>
 </file>
@@ -1404,11 +1414,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F97EDFF-72E2-4781-A226-FCA8C7C63015}">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1428,7 +1438,7 @@
     <col min="13" max="13" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>121</v>
       </c>
@@ -1465,14 +1475,23 @@
       <c r="L1" s="5" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="D3" t="s">
         <v>241</v>
@@ -1493,7 +1512,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="D4" t="s">
         <v>241</v>
@@ -1514,19 +1533,19 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>246</v>
       </c>
@@ -1534,7 +1553,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>251</v>
       </c>
@@ -1548,12 +1567,12 @@
         <v>254</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>251</v>
       </c>
@@ -1567,12 +1586,12 @@
         <v>255</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>246</v>
       </c>
@@ -1580,7 +1599,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>251</v>
       </c>
@@ -1591,7 +1610,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>251</v>
       </c>
@@ -1602,12 +1621,12 @@
         <v>277</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>251</v>
       </c>
@@ -1640,8 +1659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCA108D4-AA6D-472D-96E7-C4516EA7148E}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3926,11 +3945,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCD3AC6-97A9-4343-AD51-53B42E3E4B29}">
-  <dimension ref="A1:C120"/>
+  <dimension ref="A1:C119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3973,14 +3992,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="17"/>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" s="17"/>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="17"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="17"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B53" s="9"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B54" s="9"/>
+      <c r="B54" s="10"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B55" s="10"/>
@@ -3988,12 +4010,12 @@
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B56" s="10"/>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B57" s="10"/>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="10"/>
-      <c r="B59" s="10"/>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="10"/>
+      <c r="B58" s="10"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B60" s="10"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B61" s="10"/>
@@ -4172,11 +4194,8 @@
     <row r="119" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B119" s="10"/>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B120" s="10"/>
-    </row>
   </sheetData>
-  <sortState ref="F2:G93">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F2:G92">
     <sortCondition ref="G2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added pop-up warnings to TEST
</commit_message>
<xml_diff>
--- a/app/config/tables/TEST/forms/TEST/TEST.xlsx
+++ b/app/config/tables/TEST/forms/TEST/TEST.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE44CDE9-EBDC-4146-8880-3899EB125530}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB64C17-5B5D-4888-AA4E-E44528A0FC98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-2100" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="285">
   <si>
     <t>setting_name</t>
   </si>
@@ -886,6 +886,18 @@
   </si>
   <si>
     <t>display.constraint_message.text</t>
+  </si>
+  <si>
+    <t>{{calculates.test}}</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>data('ADA') == null</t>
+  </si>
+  <si>
+    <t>freebase.echo('Fill in the date')</t>
   </si>
 </sst>
 </file>
@@ -1414,11 +1426,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F97EDFF-72E2-4781-A226-FCA8C7C63015}">
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1546,57 +1558,54 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
       <c r="B7" t="s">
         <v>246</v>
       </c>
       <c r="C7" t="s">
-        <v>264</v>
+        <v>283</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
       <c r="D8" t="s">
         <v>251</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>246</v>
+      </c>
+      <c r="C10" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>251</v>
+      </c>
+      <c r="F11" t="s">
         <v>249</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G11" t="s">
         <v>252</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H11" t="s">
         <v>254</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D10" t="s">
-        <v>251</v>
-      </c>
-      <c r="F10" t="s">
-        <v>250</v>
-      </c>
-      <c r="G10" t="s">
-        <v>253</v>
-      </c>
-      <c r="H10" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>246</v>
-      </c>
-      <c r="C12" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -1604,26 +1613,26 @@
         <v>251</v>
       </c>
       <c r="F13" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="G13" t="s">
-        <v>275</v>
+        <v>253</v>
+      </c>
+      <c r="H13" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
-        <v>251</v>
-      </c>
-      <c r="F14" t="s">
-        <v>257</v>
-      </c>
-      <c r="G14" t="s">
-        <v>277</v>
+      <c r="B14" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>247</v>
+        <v>246</v>
+      </c>
+      <c r="C15" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -1631,22 +1640,49 @@
         <v>251</v>
       </c>
       <c r="F16" t="s">
+        <v>256</v>
+      </c>
+      <c r="G16" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>251</v>
+      </c>
+      <c r="F17" t="s">
         <v>257</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G17" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>251</v>
+      </c>
+      <c r="F19" t="s">
+        <v>257</v>
+      </c>
+      <c r="G19" t="s">
         <v>260</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H19" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1657,10 +1693,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCA108D4-AA6D-472D-96E7-C4516EA7148E}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1707,6 +1743,14 @@
       </c>
       <c r="B5" t="s">
         <v>268</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>282</v>
+      </c>
+      <c r="B6" t="s">
+        <v>284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New adata function: display
</commit_message>
<xml_diff>
--- a/app/config/tables/TEST/forms/TEST/TEST.xlsx
+++ b/app/config/tables/TEST/forms/TEST/TEST.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BC379F-0E46-49FD-B785-2B5F1322A210}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9ABDC69-90D1-4F36-8FBA-2130A6408214}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="84">
   <si>
     <t>setting_name</t>
   </si>
@@ -193,63 +193,18 @@
     <t>TEST</t>
   </si>
   <si>
-    <t>if</t>
-  </si>
-  <si>
-    <t>else</t>
-  </si>
-  <si>
-    <t>end if</t>
-  </si>
-  <si>
-    <t>lblKnown</t>
-  </si>
-  <si>
-    <t>lblUnknown</t>
-  </si>
-  <si>
     <t>note</t>
   </si>
   <si>
-    <t>OVER 2 ÅR</t>
-  </si>
-  <si>
-    <t>IKKE OVER 2 ÅR</t>
-  </si>
-  <si>
-    <t>MAS DE 2 ANOS</t>
-  </si>
-  <si>
-    <t>NAO MAS DE 2 ANOS</t>
-  </si>
-  <si>
-    <t>lblbla</t>
-  </si>
-  <si>
-    <t>lblblabla</t>
-  </si>
-  <si>
-    <t>Falsk</t>
-  </si>
-  <si>
     <t>calculation_name</t>
   </si>
   <si>
-    <t>Ingen alder…</t>
-  </si>
-  <si>
-    <t>!adate.yearUnknown(data('ADA'))</t>
-  </si>
-  <si>
     <t>display.adate.fromYear</t>
   </si>
   <si>
     <t>display.adate.toYear</t>
   </si>
   <si>
-    <t>adate.ageInYears(data('ADA'))&gt;=2</t>
-  </si>
-  <si>
     <t>ageInYears</t>
   </si>
   <si>
@@ -286,21 +241,12 @@
     <t>diffInYears</t>
   </si>
   <si>
-    <t>Differencen var: {{calculates.diffInYears}} år.</t>
-  </si>
-  <si>
     <t>constraint</t>
   </si>
   <si>
-    <t>{{calculates.test}}</t>
-  </si>
-  <si>
     <t>test</t>
   </si>
   <si>
-    <t>data('ADA') == null</t>
-  </si>
-  <si>
     <t>freebase.echo('Fill in the date')</t>
   </si>
   <si>
@@ -310,12 +256,6 @@
     <t>adate.diffInDays(data('ADA'), data('ADA2'))</t>
   </si>
   <si>
-    <t>diff in days: {{calculates.diffdays}}</t>
-  </si>
-  <si>
-    <t>diff in years: {{calculates.diffInYears}}</t>
-  </si>
-  <si>
     <t>display</t>
   </si>
   <si>
@@ -335,6 +275,15 @@
   </si>
   <si>
     <t>display: {{calculates.display}}</t>
+  </si>
+  <si>
+    <t>display:{{calculates.display}}</t>
+  </si>
+  <si>
+    <t>diff in days: &lt;b&gt;{{calculates.diffdays}}&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>diff in years: &lt;font color="red"&gt;{{calculates.diffInYears}}&lt;/font&gt;</t>
   </si>
 </sst>
 </file>
@@ -764,13 +713,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>18</v>
@@ -824,7 +773,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="E7" t="s">
         <v>19</v>
@@ -849,11 +798,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F97EDFF-72E2-4781-A226-FCA8C7C63015}">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,7 +814,7 @@
     <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="45.5703125" customWidth="1"/>
-    <col min="8" max="8" width="30" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.42578125" customWidth="1"/>
     <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="36.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.85546875" customWidth="1"/>
@@ -893,7 +842,7 @@
         <v>10</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>11</v>
@@ -905,13 +854,13 @@
         <v>40</v>
       </c>
       <c r="K1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>69</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -938,13 +887,13 @@
         <v>48</v>
       </c>
       <c r="F4" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="G4" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="H4" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -959,35 +908,35 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G7" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="H7" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G8" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="H8" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G9" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="H9" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -1001,128 +950,18 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="D12" t="s">
         <v>53</v>
       </c>
-      <c r="C12" t="s">
-        <v>88</v>
+      <c r="G12" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
-        <v>58</v>
-      </c>
-      <c r="G13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
-        <v>58</v>
-      </c>
-      <c r="F16" t="s">
-        <v>56</v>
-      </c>
-      <c r="G16" t="s">
-        <v>59</v>
-      </c>
-      <c r="H16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D18" t="s">
-        <v>58</v>
-      </c>
-      <c r="F18" t="s">
-        <v>57</v>
-      </c>
-      <c r="G18" t="s">
-        <v>60</v>
-      </c>
-      <c r="H18" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D21" t="s">
-        <v>58</v>
-      </c>
-      <c r="F21" t="s">
-        <v>63</v>
-      </c>
-      <c r="G21" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D22" t="s">
-        <v>58</v>
-      </c>
-      <c r="F22" t="s">
-        <v>64</v>
-      </c>
-      <c r="G22" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D24" t="s">
-        <v>58</v>
-      </c>
-      <c r="F24" t="s">
-        <v>64</v>
-      </c>
-      <c r="G24" t="s">
-        <v>67</v>
-      </c>
-      <c r="H24" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+      <c r="B13" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1136,7 +975,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1147,7 +986,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>32</v>
@@ -1155,58 +994,58 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="B7" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="B8" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1352,7 +1191,7 @@
         <v>15</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>16</v>
@@ -1800,7 +1639,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
Added auto "back" function in vac if warning
</commit_message>
<xml_diff>
--- a/app/config/tables/TEST/forms/TEST/TEST.xlsx
+++ b/app/config/tables/TEST/forms/TEST/TEST.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1D353E-105F-48B0-80A2-7563A843E98C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D500FB-74A0-4A4E-ACE1-42740F488F0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="86">
   <si>
     <t>setting_name</t>
   </si>
@@ -284,6 +284,12 @@
   </si>
   <si>
     <t>diff in years: &lt;font color="red"&gt;{{calculates.diffInYears}}&lt;/font&gt;</t>
+  </si>
+  <si>
+    <t>display.constraint_message.text.english</t>
+  </si>
+  <si>
+    <t>display.constraint_message.text</t>
   </si>
 </sst>
 </file>
@@ -341,6 +347,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF404040"/>
       <name val="Calibri"/>
@@ -798,11 +805,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F97EDFF-72E2-4781-A226-FCA8C7C63015}">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomLeft" activeCell="H19" sqref="B14:H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,9 +827,11 @@
     <col min="11" max="11" width="21.85546875" customWidth="1"/>
     <col min="12" max="12" width="20.28515625" customWidth="1"/>
     <col min="13" max="13" width="18.85546875" customWidth="1"/>
+    <col min="14" max="14" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="30.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>33</v>
       </c>
@@ -862,13 +871,19 @@
       <c r="M1" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>48</v>
       </c>
@@ -882,7 +897,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>48</v>
       </c>
@@ -896,17 +911,17 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>53</v>
       </c>
@@ -917,7 +932,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>53</v>
       </c>
@@ -928,7 +943,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>53</v>
       </c>
@@ -939,17 +954,17 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>53</v>
       </c>
@@ -960,7 +975,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>13</v>
       </c>
@@ -974,8 +989,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCA108D4-AA6D-472D-96E7-C4516EA7148E}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>